<commit_message>
Output files that were changed. Dont know how to ignore
</commit_message>
<xml_diff>
--- a/excel_files/Comparison - Ancestor 1 & CP001666.xlsx
+++ b/excel_files/Comparison - Ancestor 1 & CP001666.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="100">
   <si>
     <t>Ancestor 1</t>
   </si>
@@ -23,88 +23,88 @@
     <t>CP001666</t>
   </si>
   <si>
+    <t>[Ser_UCA, Ser_AGC, Ser_UCA, Ser_AGC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arg_CGU</t>
+  </si>
+  <si>
+    <t>[Leu_UUA, Met_AUG, Met_AUG, Leu_UUA, Met_AUG, Met_AUG, Leu_UUA, Met_AUG, Leu_UUA]</t>
+  </si>
+  <si>
+    <t>[Asn_AAC, Asn_AAC, Asn_AAC]</t>
+  </si>
+  <si>
+    <t>[16S, Ala_GCA, Ile_AUC, 23S, 5S, Phe_UUC, Cys_UGC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thr_ACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leu_CUA</t>
+  </si>
+  <si>
+    <t>[Pro_CCA, Gly_GGA, Arg_AGA, Pro_CCA, Gly_GGA, Arg_AGA, His_CAC, Gln_CAA, Lys_AAA, Leu_CUA, Gly_GGC, Gly_GGA, Lys_AAG, Gln_CAA, Lys_AAA, Leu_CUA, Gly_GGC, Gly_GGA, Arg_CGA]</t>
+  </si>
+  <si>
+    <t>[Arg_AGA, Gly_GGA, Gly_GGA, Arg_AGA, His_CAC, Gln_CAA, Lys_AAA]</t>
+  </si>
+  <si>
+    <t>[16S, Ile_AUC, 23S, Asn_AAC]</t>
+  </si>
+  <si>
+    <t>[Tyr_UAC, Val_GUA, Thr_ACA, Tyr_UAC, Val_GUA, Thr_ACA, Tyr_UAC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trp_UGG</t>
+  </si>
+  <si>
+    <t>[16S, 23S, 5S]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gln_CAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leu_CUU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Cys_UGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leu_UUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Glu_GAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pro_CCA</t>
+  </si>
+  <si>
+    <t>-[Phe_UUC, 5S]</t>
+  </si>
+  <si>
+    <t>-[Lys_AAA, Lys_AAG, 5S, 23S, 16S]</t>
+  </si>
+  <si>
+    <t>-[5S, 23S, 16S]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Ser_UCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Arg_AGG</t>
+  </si>
+  <si>
+    <t>-[Asp_GAC, Val_GUA, Glu_GAA, Thr_ACA, Asp_GAC, Val_GUA, Glu_GAA, Thr_ACA, Asp_GAC, Val_GUA, Glu_GAA]</t>
+  </si>
+  <si>
     <t>[16S, 23S, 5S, Met_AUG, Ala_GCA]</t>
   </si>
   <si>
-    <t>[Ser_UCA, Ser_AGC, Ser_UCA, Ser_AGC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Arg_CGU</t>
-  </si>
-  <si>
-    <t>[Leu_UUA, Met_AUG, Met_AUG, Leu_UUA, Met_AUG, Met_AUG, Leu_UUA, Met_AUG, Leu_UUA]</t>
-  </si>
-  <si>
-    <t>[Asn_AAC, Asn_AAC, Asn_AAC]</t>
-  </si>
-  <si>
-    <t>[16S, Ala_GCA, Ile_AUC, 23S, 5S, Phe_UUC, Cys_UGC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thr_ACC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Leu_CUA</t>
-  </si>
-  <si>
-    <t>[Pro_CCA, Gly_GGA, Arg_AGA, Pro_CCA, Gly_GGA, Arg_AGA, His_CAC, Gln_CAA, Lys_AAA, Leu_CUA, Gly_GGC, Gly_GGA, Lys_AAG, Gln_CAA, Lys_AAA, Leu_CUA, Gly_GGC, Gly_GGA, Arg_CGA]</t>
-  </si>
-  <si>
-    <t>[Arg_AGA, Gly_GGA, Gly_GGA, Arg_AGA, His_CAC, Gln_CAA, Lys_AAA]</t>
-  </si>
-  <si>
-    <t>[16S, Ile_AUC, 23S, Asn_AAC]</t>
-  </si>
-  <si>
-    <t>[Tyr_UAC, Val_GUA, Thr_ACA, Tyr_UAC, Val_GUA, Thr_ACA, Tyr_UAC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trp_UGG</t>
-  </si>
-  <si>
-    <t>[16S, 23S, 5S]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gln_CAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Leu_CUU</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -Cys_UGC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Leu_UUG</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Glu_GAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pro_CCA</t>
-  </si>
-  <si>
-    <t>-[Phe_UUC, 5S]</t>
-  </si>
-  <si>
-    <t>-[Ala_GCA, Met_AUG, 5S, 23S, 16S]</t>
-  </si>
-  <si>
-    <t>-[Lys_AAA, Lys_AAG, 5S, 23S, 16S]</t>
-  </si>
-  <si>
-    <t>-[5S, 23S, 16S]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -Ser_UCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -Arg_AGG</t>
-  </si>
-  <si>
-    <t>-[5S, 23S, 16S, 5S, 23S, Ala_GCA, 16S]</t>
-  </si>
-  <si>
-    <t>-[Asp_GAC, Val_GUA, Glu_GAA, Thr_ACA, Asp_GAC, Val_GUA, Glu_GAA, Thr_ACA, Asp_GAC, Val_GUA, Glu_GAA]</t>
+    <t>-[Ala_GCA, Met_AUG, 5S, 23S, 16S, 5S, 23S, 16S]</t>
+  </si>
+  <si>
+    <t>-[5S, 23S, 16S, 5S, 23S, 16S, 5S, 23S, Ala_GCA, 16S]</t>
   </si>
   <si>
     <t>[16S, 23S, 5S, Met_AUG]</t>
@@ -194,94 +194,127 @@
     <t xml:space="preserve"> -Thr_ACG</t>
   </si>
   <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>-999</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>19.0</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>13.0</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>22.5</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>23.0</t>
+  </si>
+  <si>
+    <t>20.5</t>
+  </si>
+  <si>
+    <t>19.5</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>24.0</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>10.0*</t>
+  </si>
+  <si>
+    <t>26.0</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>2.0*</t>
+  </si>
+  <si>
+    <t>0*</t>
+  </si>
+  <si>
     <t>1.0*</t>
   </si>
   <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>-999</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>4.0</t>
+    <t>0.0*</t>
+  </si>
+  <si>
+    <t>17.0</t>
+  </si>
+  <si>
+    <t>11.5</t>
   </si>
   <si>
     <t>3.0*</t>
   </si>
   <si>
-    <t>15.0</t>
-  </si>
-  <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>14.5</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>19.0</t>
-  </si>
-  <si>
-    <t>18.5</t>
-  </si>
-  <si>
-    <t>18.0</t>
-  </si>
-  <si>
-    <t>16.0</t>
-  </si>
-  <si>
-    <t>7.5*</t>
-  </si>
-  <si>
-    <t>6.5</t>
-  </si>
-  <si>
-    <t>11.5</t>
-  </si>
-  <si>
-    <t>2.0*</t>
-  </si>
-  <si>
-    <t>0*</t>
-  </si>
-  <si>
-    <t>0.0*</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>14.0</t>
-  </si>
-  <si>
-    <t>11.0</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>10.5</t>
+    <t>20.0</t>
   </si>
 </sst>
 </file>
@@ -678,7 +711,7 @@
         <v>43</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
         <v>44</v>
@@ -730,98 +763,98 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD3" t="s">
         <v>63</v>
       </c>
-      <c r="M3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" t="s">
-        <v>62</v>
-      </c>
-      <c r="S3" t="s">
-        <v>60</v>
-      </c>
-      <c r="T3" t="s">
-        <v>61</v>
-      </c>
-      <c r="U3" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" t="s">
-        <v>61</v>
-      </c>
-      <c r="W3" t="s">
-        <v>60</v>
-      </c>
-      <c r="X3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>60</v>
-      </c>
       <c r="AE3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AG3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:33">
@@ -829,97 +862,97 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="O4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Y4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="AC4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AE4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AG4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -927,97 +960,97 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="O5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="P5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="S5" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="T5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="Y5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="AB5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="AC5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="AE5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF5" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="AG5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -1028,97 +1061,97 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="K6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="N6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="O6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="S6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="T6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X6" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="Y6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="AB6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AE6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AG6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -1126,97 +1159,97 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
         <v>63</v>
       </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
         <v>60</v>
       </c>
-      <c r="K7" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" t="s">
-        <v>63</v>
-      </c>
       <c r="M7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N7" t="s">
         <v>60</v>
       </c>
       <c r="O7" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" t="s">
+        <v>75</v>
+      </c>
+      <c r="S7" t="s">
+        <v>65</v>
+      </c>
+      <c r="T7" t="s">
+        <v>62</v>
+      </c>
+      <c r="U7" t="s">
+        <v>62</v>
+      </c>
+      <c r="V7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W7" t="s">
+        <v>66</v>
+      </c>
+      <c r="X7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA7" t="s">
         <v>63</v>
       </c>
-      <c r="P7" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" t="s">
-        <v>73</v>
-      </c>
-      <c r="S7" t="s">
-        <v>73</v>
-      </c>
-      <c r="T7" t="s">
-        <v>61</v>
-      </c>
-      <c r="U7" t="s">
-        <v>61</v>
-      </c>
-      <c r="V7" t="s">
-        <v>61</v>
-      </c>
-      <c r="W7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>73</v>
-      </c>
       <c r="AB7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="AC7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD7" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="AE7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF7" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="AG7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -1224,97 +1257,97 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="M8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
       </c>
       <c r="O8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="T8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="X8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Y8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AB8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AC8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AE8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AG8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -1322,97 +1355,97 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AG9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -1420,97 +1453,97 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="K10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="M10" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="N10" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="P10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R10" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="S10" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="T10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W10" t="s">
-        <v>61</v>
-      </c>
-      <c r="X10" t="s">
-        <v>61</v>
+        <v>83</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="Y10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA10" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="AB10" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="AC10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD10" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="AE10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF10" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="AG10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -1518,97 +1551,97 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="M11" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="O11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="P11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="S11" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="T11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W11" t="s">
-        <v>76</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
+      </c>
+      <c r="X11" t="s">
+        <v>69</v>
       </c>
       <c r="Y11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA11" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="AB11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="AC11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD11" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="AE11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AG11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -1616,97 +1649,97 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
-        <v>79</v>
-      </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" t="s">
+        <v>91</v>
+      </c>
+      <c r="M12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>62</v>
+      </c>
+      <c r="R12" t="s">
+        <v>60</v>
+      </c>
+      <c r="S12" t="s">
+        <v>66</v>
+      </c>
+      <c r="T12" t="s">
+        <v>62</v>
+      </c>
+      <c r="U12" t="s">
+        <v>62</v>
+      </c>
+      <c r="V12" t="s">
+        <v>62</v>
+      </c>
+      <c r="W12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF12" t="s">
         <v>68</v>
       </c>
-      <c r="H12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" t="s">
-        <v>66</v>
-      </c>
-      <c r="M12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O12" t="s">
-        <v>66</v>
-      </c>
-      <c r="P12" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>61</v>
-      </c>
-      <c r="R12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" t="s">
-        <v>68</v>
-      </c>
-      <c r="T12" t="s">
-        <v>61</v>
-      </c>
-      <c r="U12" t="s">
-        <v>61</v>
-      </c>
-      <c r="V12" t="s">
-        <v>61</v>
-      </c>
-      <c r="W12" t="s">
-        <v>79</v>
-      </c>
-      <c r="X12" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>66</v>
-      </c>
       <c r="AG12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -1714,97 +1747,97 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
         <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
-      </c>
-      <c r="J13" t="s">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="K13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L13" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="M13" t="s">
         <v>63</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>81</v>
+      <c r="N13" t="s">
+        <v>70</v>
       </c>
       <c r="O13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="P13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="S13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W13" t="s">
         <v>63</v>
       </c>
       <c r="X13" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="Y13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA13" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="AB13" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="AC13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD13" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="AE13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="AG13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -1812,391 +1845,391 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="T14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="X14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="Z14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA14" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="AB14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AE14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AG14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:33">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="Z15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AG15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:33">
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
-        <v>61</v>
+      <c r="C16" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="J16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N16" t="s">
-        <v>61</v>
-      </c>
-      <c r="O16" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="P16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q16" t="s">
-        <v>61</v>
-      </c>
-      <c r="R16" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="S16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="T16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W16" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="X16" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>62</v>
       </c>
       <c r="Z16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA16" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="AB16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AE16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF16" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AG16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:33">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>59</v>
+      <c r="C17" t="s">
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" t="s">
+        <v>62</v>
       </c>
       <c r="J17" t="s">
-        <v>60</v>
-      </c>
-      <c r="K17" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="M17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="N17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="O17" t="s">
+        <v>62</v>
       </c>
       <c r="P17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q17" t="s">
-        <v>61</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
+      </c>
+      <c r="R17" t="s">
+        <v>62</v>
       </c>
       <c r="S17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="T17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Y17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="AB17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="AC17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AE17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF17" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AG17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -2204,97 +2237,97 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>61</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
+      </c>
+      <c r="K18" t="s">
+        <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AG18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -2302,97 +2335,97 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AG19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:33">
@@ -2400,97 +2433,97 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T20" t="s">
-        <v>61</v>
-      </c>
-      <c r="U20" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="V20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AG20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -2498,97 +2531,97 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S21" t="s">
-        <v>61</v>
-      </c>
-      <c r="T21" t="s">
-        <v>61</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="U21" t="s">
+        <v>62</v>
       </c>
       <c r="V21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AG21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:33">
@@ -2596,97 +2629,97 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S22" t="s">
-        <v>61</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
+      </c>
+      <c r="T22" t="s">
+        <v>62</v>
       </c>
       <c r="U22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AG22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:33">
@@ -2694,97 +2727,97 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="J23" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="K23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L23" t="s">
-        <v>61</v>
-      </c>
-      <c r="M23" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="N23" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="O23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="P23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S23" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="T23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="X23" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="Y23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="AB23" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AC23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD23" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AE23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AG23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="2:33">
@@ -2792,97 +2825,97 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" t="s">
-        <v>73</v>
+        <v>62</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" t="s">
+        <v>77</v>
+      </c>
+      <c r="M24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N24" t="s">
+        <v>77</v>
+      </c>
+      <c r="O24" t="s">
         <v>60</v>
       </c>
-      <c r="K24" t="s">
-        <v>61</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="P24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>62</v>
+      </c>
+      <c r="R24" t="s">
+        <v>91</v>
+      </c>
+      <c r="S24" t="s">
+        <v>64</v>
+      </c>
+      <c r="T24" t="s">
+        <v>62</v>
+      </c>
+      <c r="U24" t="s">
+        <v>62</v>
+      </c>
+      <c r="V24" t="s">
+        <v>62</v>
+      </c>
+      <c r="W24" t="s">
         <v>63</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="N24" t="s">
-        <v>60</v>
-      </c>
-      <c r="O24" t="s">
-        <v>63</v>
-      </c>
-      <c r="P24" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>61</v>
-      </c>
-      <c r="R24" t="s">
-        <v>73</v>
-      </c>
-      <c r="S24" t="s">
-        <v>73</v>
-      </c>
-      <c r="T24" t="s">
-        <v>61</v>
-      </c>
-      <c r="U24" t="s">
-        <v>61</v>
-      </c>
-      <c r="V24" t="s">
-        <v>61</v>
-      </c>
-      <c r="W24" t="s">
-        <v>73</v>
-      </c>
       <c r="X24" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD24" t="s">
         <v>65</v>
       </c>
-      <c r="Y24" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>60</v>
-      </c>
       <c r="AE24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AG24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="2:33">
@@ -2890,97 +2923,97 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25" t="s">
         <v>59</v>
       </c>
-      <c r="D25" t="s">
+      <c r="K25" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" t="s">
         <v>60</v>
       </c>
-      <c r="E25" t="s">
+      <c r="M25" t="s">
         <v>60</v>
       </c>
-      <c r="F25" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" t="s">
-        <v>62</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="N25" t="s">
         <v>60</v>
       </c>
-      <c r="K25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L25" t="s">
-        <v>63</v>
-      </c>
-      <c r="M25" t="s">
-        <v>63</v>
-      </c>
-      <c r="N25" t="s">
-        <v>63</v>
-      </c>
       <c r="O25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P25" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>62</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S25" t="s">
         <v>64</v>
       </c>
-      <c r="P25" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>61</v>
-      </c>
-      <c r="R25" t="s">
-        <v>62</v>
-      </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
+        <v>62</v>
+      </c>
+      <c r="U25" t="s">
+        <v>62</v>
+      </c>
+      <c r="V25" t="s">
+        <v>62</v>
+      </c>
+      <c r="W25" t="s">
+        <v>66</v>
+      </c>
+      <c r="X25" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB25" t="s">
         <v>60</v>
       </c>
-      <c r="T25" t="s">
-        <v>61</v>
-      </c>
-      <c r="U25" t="s">
-        <v>61</v>
-      </c>
-      <c r="V25" t="s">
-        <v>61</v>
-      </c>
-      <c r="W25" t="s">
-        <v>60</v>
-      </c>
-      <c r="X25" t="s">
+      <c r="AC25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF25" t="s">
         <v>65</v>
       </c>
-      <c r="Y25" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>66</v>
-      </c>
       <c r="AG25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="2:33">
@@ -2991,16 +3024,16 @@
         <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
       </c>
       <c r="H26" t="s">
         <v>62</v>
@@ -3009,174 +3042,174 @@
         <v>62</v>
       </c>
       <c r="J26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O26" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="P26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R26" t="s">
         <v>62</v>
       </c>
       <c r="S26" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="T26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="X26" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="Y26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AB26" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="AC26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AE26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AG26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:33">
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>59</v>
+      <c r="C27" t="s">
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="G27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" t="s">
+        <v>62</v>
       </c>
       <c r="J27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L27" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="M27" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="N27" t="s">
-        <v>73</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="O27" t="s">
+        <v>62</v>
       </c>
       <c r="P27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q27" t="s">
-        <v>61</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
+      </c>
+      <c r="R27" t="s">
+        <v>62</v>
       </c>
       <c r="S27" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="T27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Y27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA27" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="AB27" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="AC27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AE27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AG27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -3184,195 +3217,195 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
+      </c>
+      <c r="F28" t="s">
+        <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="J28" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L28" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="M28" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="N28" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="O28" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="P28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="S28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="T28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W28" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="X28" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="Y28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA28" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="AB28" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="AC28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD28" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="AE28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF28" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="AG28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="2:33">
       <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>61</v>
+      <c r="C29" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L29" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="M29" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="N29" t="s">
-        <v>61</v>
-      </c>
-      <c r="O29" t="s">
-        <v>61</v>
+        <v>77</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="P29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R29" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="S29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="X29" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="Y29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="AC29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AE29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF29" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="AG29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="2:33">
@@ -3380,97 +3413,97 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J30" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" t="s">
+        <v>59</v>
+      </c>
+      <c r="O30" t="s">
+        <v>64</v>
+      </c>
+      <c r="P30" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>62</v>
+      </c>
+      <c r="R30" t="s">
+        <v>77</v>
+      </c>
+      <c r="S30" t="s">
         <v>68</v>
       </c>
-      <c r="N30" t="s">
-        <v>63</v>
-      </c>
-      <c r="O30" t="s">
-        <v>63</v>
-      </c>
-      <c r="P30" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>61</v>
-      </c>
-      <c r="R30" t="s">
-        <v>63</v>
-      </c>
-      <c r="S30" t="s">
-        <v>66</v>
-      </c>
       <c r="T30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W30" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="X30" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA30" t="s">
         <v>65</v>
       </c>
-      <c r="Y30" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>66</v>
-      </c>
       <c r="AB30" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="AC30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AE30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF30" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="AG30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="2:33">
@@ -3478,97 +3511,97 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="H31" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="I31" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="J31" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" t="s">
+        <v>59</v>
+      </c>
+      <c r="M31" t="s">
+        <v>65</v>
+      </c>
+      <c r="N31" t="s">
+        <v>59</v>
+      </c>
+      <c r="O31" t="s">
+        <v>59</v>
+      </c>
+      <c r="P31" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>62</v>
+      </c>
+      <c r="R31" t="s">
+        <v>66</v>
+      </c>
+      <c r="S31" t="s">
+        <v>70</v>
+      </c>
+      <c r="T31" t="s">
+        <v>62</v>
+      </c>
+      <c r="U31" t="s">
+        <v>62</v>
+      </c>
+      <c r="V31" t="s">
+        <v>62</v>
+      </c>
+      <c r="W31" t="s">
+        <v>71</v>
+      </c>
+      <c r="X31" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA31" t="s">
         <v>69</v>
       </c>
-      <c r="K31" t="s">
-        <v>61</v>
-      </c>
-      <c r="L31" t="s">
-        <v>86</v>
-      </c>
-      <c r="M31" t="s">
-        <v>86</v>
-      </c>
-      <c r="N31" t="s">
-        <v>86</v>
-      </c>
-      <c r="O31" t="s">
-        <v>86</v>
-      </c>
-      <c r="P31" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>61</v>
-      </c>
-      <c r="R31" t="s">
-        <v>86</v>
-      </c>
-      <c r="S31" t="s">
-        <v>86</v>
-      </c>
-      <c r="T31" t="s">
-        <v>61</v>
-      </c>
-      <c r="U31" t="s">
-        <v>61</v>
-      </c>
-      <c r="V31" t="s">
-        <v>61</v>
-      </c>
-      <c r="W31" t="s">
-        <v>87</v>
-      </c>
-      <c r="X31" t="s">
+      <c r="AB31" t="s">
         <v>65</v>
       </c>
-      <c r="Y31" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>86</v>
-      </c>
       <c r="AC31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD31" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="AE31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF31" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="AG31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3636,7 +3669,7 @@
         <v>43</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
         <v>44</v>
@@ -3749,7 +3782,7 @@
     </row>
     <row r="15" spans="1:33">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:33">

</xml_diff>